<commit_message>
Updated the model to assume that we have 30 fb-1 level (tunable parameter) operation now
</commit_message>
<xml_diff>
--- a/USTier2ComputingProjections.xlsx
+++ b/USTier2ComputingProjections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Year</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>2016 is actually scary - we are going to not buy :(</t>
+  </si>
+  <si>
+    <t>2015 MC Level (fb)</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -277,24 +280,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -663,66 +666,67 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="9" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="7" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
     </row>
     <row r="3" spans="1:17">
       <c r="B3" t="s">
@@ -761,7 +765,7 @@
       <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="7" t="s">
         <v>43</v>
       </c>
       <c r="O3" t="s">
@@ -770,7 +774,7 @@
       <c r="P3" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -791,37 +795,37 @@
       <c r="E4">
         <v>15000</v>
       </c>
-      <c r="F4" s="5">
-        <f>(C4+10)*C15*C16*C19*C20/C21</f>
-        <v>0.308</v>
-      </c>
-      <c r="G4" s="5">
-        <f>(C4+10)*C15*C16*C17*C18/C21</f>
-        <v>0.77000000000000013</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="6">
+      <c r="F4" s="4">
+        <f>(C4+C13)*C15*C16*C19*C20/C21</f>
+        <v>3.8148</v>
+      </c>
+      <c r="G4" s="4">
+        <f>(C4+C13)*C15*C16*C17*C18/C21</f>
+        <v>9.5370000000000008</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5">
         <f>65200/7</f>
         <v>9314.2857142857138</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>2</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="10">
         <v>118</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="10">
         <v>56</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13">
+      <c r="N4" s="10"/>
+      <c r="O4" s="10">
         <v>118</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="10">
         <v>56</v>
       </c>
-      <c r="Q4" s="13"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1">
@@ -835,60 +839,60 @@
         <v>40</v>
       </c>
       <c r="D5">
-        <f>D4*B5/10</f>
-        <v>54000</v>
-      </c>
-      <c r="E5">
-        <f>E4*C5/10</f>
-        <v>60000</v>
-      </c>
-      <c r="F5" s="6">
+        <f>D4*B5/C13</f>
+        <v>18000</v>
+      </c>
+      <c r="E5" s="5">
+        <f>E4*C5/C13</f>
+        <v>20000</v>
+      </c>
+      <c r="F5" s="5">
         <f>(C5*C14)*C15*C16*C19*C20/C21</f>
-        <v>1.76</v>
+        <v>8.9760000000000009</v>
       </c>
       <c r="G5">
         <f>(C5*C14)*C15*C16*C17*C18/C21</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H5" s="6">
+        <v>22.44</v>
+      </c>
+      <c r="H5" s="5">
         <f>J5-J4</f>
-        <v>6971.4285714285725</v>
-      </c>
-      <c r="I5" s="5">
+        <v>-3885.7142857142853</v>
+      </c>
+      <c r="I5" s="4">
         <f>K5-K4</f>
-        <v>-1.1200000000000001</v>
-      </c>
-      <c r="J5" s="6">
-        <f>(D5+E5)/7</f>
-        <v>16285.714285714286</v>
-      </c>
-      <c r="K5" s="5">
-        <f>SUM(F5:G5)/7</f>
-        <v>0.88</v>
-      </c>
-      <c r="L5" s="13">
+        <v>2.4880000000000004</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" ref="J5:J11" si="0">(D5+E5)/7</f>
+        <v>5428.5714285714284</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" ref="K5:K11" si="1">SUM(F5:G5)/7</f>
+        <v>4.4880000000000004</v>
+      </c>
+      <c r="L5" s="10">
         <f>L4*0.9</f>
         <v>106.2</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="10">
         <f>M4*0.9</f>
         <v>50.4</v>
       </c>
-      <c r="N5" s="13">
-        <f>((H5*L5)+(I5*2*1000*M5))</f>
-        <v>627469.71428571444</v>
-      </c>
-      <c r="O5" s="13">
+      <c r="N5" s="10">
+        <f t="shared" ref="N5:N11" si="2">((H5*L5)+(I5*2*1000*M5))</f>
+        <v>-161872.45714285705</v>
+      </c>
+      <c r="O5" s="10">
         <f>O4*0.8</f>
         <v>94.4</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="10">
         <f>P4*0.8</f>
         <v>44.800000000000004</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="10">
         <f>((H5*O5)+(I5*2*1000*P5))</f>
-        <v>557750.85714285728</v>
+        <v>-143886.6285714285</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -899,64 +903,64 @@
         <v>40</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C11" si="0">C5+B6</f>
+        <f t="shared" ref="C6:C11" si="3">C5+B6</f>
         <v>80</v>
       </c>
       <c r="D6">
-        <f>D4*B6/10</f>
-        <v>60000</v>
-      </c>
-      <c r="E6">
-        <f>E4*C6/10</f>
-        <v>120000</v>
-      </c>
-      <c r="F6" s="6">
+        <f>D4*B6/C13</f>
+        <v>20000</v>
+      </c>
+      <c r="E6" s="5">
+        <f>E4*C6/C13</f>
+        <v>40000</v>
+      </c>
+      <c r="F6" s="5">
         <f>(C6*C14)*C15*C16*C19*C20/C21</f>
-        <v>3.52</v>
+        <v>17.952000000000002</v>
       </c>
       <c r="G6">
         <f>(C6*C14)*C15*C16*C17*C18/C21</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="H6" s="6">
-        <f t="shared" ref="H6:H11" si="1">J6-J5</f>
-        <v>9428.5714285714275</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" ref="I6:I11" si="2">K6-K5</f>
-        <v>0.88</v>
-      </c>
-      <c r="J6" s="6">
-        <f>(D6+E6)/7</f>
-        <v>25714.285714285714</v>
-      </c>
-      <c r="K6" s="5">
-        <f>SUM(F6:G6)/7</f>
-        <v>1.76</v>
-      </c>
-      <c r="L6" s="13">
+        <v>44.88</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ref="H6:H11" si="4">J6-J5</f>
+        <v>3142.8571428571422</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I11" si="5">K6-K5</f>
+        <v>4.4880000000000004</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="0"/>
+        <v>8571.4285714285706</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
+        <v>8.9760000000000009</v>
+      </c>
+      <c r="L6" s="10">
         <f>L5*0.9</f>
         <v>95.58</v>
       </c>
-      <c r="M6" s="13">
-        <f t="shared" ref="M6:M11" si="3">M5*0.9</f>
+      <c r="M6" s="10">
+        <f t="shared" ref="M6:M11" si="6">M5*0.9</f>
         <v>45.36</v>
       </c>
-      <c r="N6" s="13">
-        <f>((H6*L6)+(I6*2*1000*M6))</f>
-        <v>981016.45714285702</v>
-      </c>
-      <c r="O6" s="13">
-        <f t="shared" ref="O6:O11" si="4">O5*0.8</f>
+      <c r="N6" s="10">
+        <f t="shared" si="2"/>
+        <v>707545.64571428555</v>
+      </c>
+      <c r="O6" s="10">
+        <f t="shared" ref="O6:O11" si="7">O5*0.8</f>
         <v>75.52000000000001</v>
       </c>
-      <c r="P6" s="13">
-        <f t="shared" ref="P6:P11" si="5">P5*0.8</f>
+      <c r="P6" s="10">
+        <f t="shared" ref="P6:P11" si="8">P5*0.8</f>
         <v>35.840000000000003</v>
       </c>
-      <c r="Q6" s="13">
-        <f t="shared" ref="Q6:Q11" si="6">((H6*O6)+(I6*2*1000*P6))</f>
-        <v>775124.11428571434</v>
+      <c r="Q6" s="10">
+        <f t="shared" ref="Q6:Q11" si="9">((H6*O6)+(I6*2*1000*P6))</f>
+        <v>559048.41142857145</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -967,64 +971,64 @@
         <v>40</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="D7">
-        <f>D4*B7/10</f>
+        <f>D4*B7/C13</f>
+        <v>20000</v>
+      </c>
+      <c r="E7" s="5">
+        <f>E4*C7/C13</f>
         <v>60000</v>
       </c>
-      <c r="E7">
-        <f>E4*C7/10</f>
-        <v>180000</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f>(C7*C14)*C15*C16*C19*C20/C21</f>
-        <v>5.28</v>
+        <v>26.928000000000001</v>
       </c>
       <c r="G7">
         <f>(C7*C14)*C15*C16*C17*C18/C21</f>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="H7" s="6">
+        <v>67.320000000000007</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="4"/>
+        <v>2857.1428571428587</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="5"/>
+        <v>4.4879999999999995</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>11428.571428571429</v>
+      </c>
+      <c r="K7" s="4">
         <f t="shared" si="1"/>
-        <v>8571.4285714285688</v>
-      </c>
-      <c r="I7" s="5">
+        <v>13.464</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" ref="L7:L11" si="10">L6*0.9</f>
+        <v>86.022000000000006</v>
+      </c>
+      <c r="M7" s="10">
+        <f t="shared" si="6"/>
+        <v>40.823999999999998</v>
+      </c>
+      <c r="N7" s="10">
         <f t="shared" si="2"/>
-        <v>0.88000000000000012</v>
-      </c>
-      <c r="J7" s="6">
-        <f>(D7+E7)/7</f>
-        <v>34285.714285714283</v>
-      </c>
-      <c r="K7" s="5">
-        <f>SUM(F7:G7)/7</f>
-        <v>2.64</v>
-      </c>
-      <c r="L7" s="13">
-        <f t="shared" ref="L7:L11" si="7">L6*0.9</f>
-        <v>86.022000000000006</v>
-      </c>
-      <c r="M7" s="13">
-        <f t="shared" si="3"/>
-        <v>40.823999999999998</v>
-      </c>
-      <c r="N7" s="13">
-        <f>((H7*L7)+(I7*2*1000*M7))</f>
-        <v>809181.6685714284</v>
-      </c>
-      <c r="O7" s="13">
-        <f t="shared" si="4"/>
+        <v>612213.366857143</v>
+      </c>
+      <c r="O7" s="10">
+        <f t="shared" si="7"/>
         <v>60.416000000000011</v>
       </c>
-      <c r="P7" s="13">
-        <f t="shared" si="5"/>
+      <c r="P7" s="10">
+        <f t="shared" si="8"/>
         <v>28.672000000000004</v>
       </c>
-      <c r="Q7" s="13">
-        <f t="shared" si="6"/>
-        <v>568314.14857142849</v>
+      <c r="Q7" s="10">
+        <f t="shared" si="9"/>
+        <v>429977.01485714305</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1035,64 +1039,64 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8" si="8">D7*B8/B7</f>
+        <f t="shared" ref="D8" si="11">D7*B8/B7</f>
         <v>0</v>
       </c>
-      <c r="E8">
-        <f>E4*C8/10</f>
-        <v>180000</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="E8" s="5">
+        <f>E4*C8/C13</f>
+        <v>60000</v>
+      </c>
+      <c r="F8" s="5">
         <f>(C8*C14)*C15*C16*C19*C20/C21</f>
-        <v>5.28</v>
+        <v>26.928000000000001</v>
       </c>
       <c r="G8">
         <f>(C8*C14)*C15*C16*C17*C18/C21</f>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="H8" s="6">
+        <v>67.320000000000007</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="4"/>
+        <v>-2857.1428571428587</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>8571.4285714285706</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" si="1"/>
-        <v>-8571.4285714285688</v>
-      </c>
-      <c r="I8" s="5">
+        <v>13.464</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="10"/>
+        <v>77.419800000000009</v>
+      </c>
+      <c r="M8" s="10">
+        <f t="shared" si="6"/>
+        <v>36.741599999999998</v>
+      </c>
+      <c r="N8" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <f>(D8+E8)/7</f>
-        <v>25714.285714285714</v>
-      </c>
-      <c r="K8" s="5">
-        <f>SUM(F8:G8)/7</f>
-        <v>2.64</v>
-      </c>
-      <c r="L8" s="13">
+        <v>-221199.42857142873</v>
+      </c>
+      <c r="O8" s="10">
         <f t="shared" si="7"/>
-        <v>77.419800000000009</v>
-      </c>
-      <c r="M8" s="13">
-        <f t="shared" si="3"/>
-        <v>36.741599999999998</v>
-      </c>
-      <c r="N8" s="13">
-        <f>((H8*L8)+(I8*2*1000*M8))</f>
-        <v>-663598.28571428556</v>
-      </c>
-      <c r="O8" s="13">
-        <f t="shared" si="4"/>
         <v>48.332800000000013</v>
       </c>
-      <c r="P8" s="13">
-        <f t="shared" si="5"/>
+      <c r="P8" s="10">
+        <f t="shared" si="8"/>
         <v>22.937600000000003</v>
       </c>
-      <c r="Q8" s="13">
-        <f t="shared" si="6"/>
-        <v>-414281.14285714284</v>
+      <c r="Q8" s="10">
+        <f t="shared" si="9"/>
+        <v>-138093.71428571441</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1103,62 +1107,62 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9">
-        <f>E4*C9/10</f>
-        <v>180000</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="E9" s="5">
+        <f>E4*C9/C13</f>
+        <v>60000</v>
+      </c>
+      <c r="F9" s="5">
         <f>(C9*C14)*C15*C16*C19*C20/C21</f>
-        <v>5.28</v>
+        <v>26.928000000000001</v>
       </c>
       <c r="G9">
         <f>(C9*C14)*C15*C16*C17*C18/C21</f>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="H9" s="6">
+        <v>67.320000000000007</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>8571.4285714285706</v>
+      </c>
+      <c r="K9" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
+        <v>13.464</v>
+      </c>
+      <c r="L9" s="10">
+        <f t="shared" si="10"/>
+        <v>69.677820000000011</v>
+      </c>
+      <c r="M9" s="10">
+        <f t="shared" si="6"/>
+        <v>33.067439999999998</v>
+      </c>
+      <c r="N9" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J9" s="6">
-        <f>(D9+E9)/7</f>
-        <v>25714.285714285714</v>
-      </c>
-      <c r="K9" s="5">
-        <f>SUM(F9:G9)/7</f>
-        <v>2.64</v>
-      </c>
-      <c r="L9" s="13">
+      <c r="O9" s="10">
         <f t="shared" si="7"/>
-        <v>69.677820000000011</v>
-      </c>
-      <c r="M9" s="13">
-        <f t="shared" si="3"/>
-        <v>33.067439999999998</v>
-      </c>
-      <c r="N9" s="13">
-        <f>((H9*L9)+(I9*2*1000*M9))</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="13">
-        <f t="shared" si="4"/>
         <v>38.666240000000016</v>
       </c>
-      <c r="P9" s="13">
-        <f t="shared" si="5"/>
+      <c r="P9" s="10">
+        <f t="shared" si="8"/>
         <v>18.350080000000002</v>
       </c>
-      <c r="Q9" s="13">
-        <f t="shared" si="6"/>
+      <c r="Q9" s="10">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1170,64 +1174,64 @@
         <v>80</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="D10">
-        <f>D4*B10/10</f>
-        <v>120000</v>
-      </c>
-      <c r="E10">
-        <f>E4*C10/10</f>
-        <v>300000</v>
-      </c>
-      <c r="F10" s="6">
+        <f>D4*B10/C13</f>
+        <v>40000</v>
+      </c>
+      <c r="E10" s="5">
+        <f>E4*C10/C13</f>
+        <v>100000</v>
+      </c>
+      <c r="F10" s="5">
         <f>(C10*C14)*C15*C16*C19*C20/C21</f>
-        <v>8.8000000000000007</v>
+        <v>44.88</v>
       </c>
       <c r="G10">
         <f>(C10*C14)*C15*C16*C17*C18/C21</f>
-        <v>22</v>
-      </c>
-      <c r="H10" s="6">
+        <v>112.20000000000002</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="4"/>
+        <v>11428.571428571429</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="5"/>
+        <v>8.9760000000000009</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="K10" s="4">
         <f t="shared" si="1"/>
-        <v>34285.71428571429</v>
-      </c>
-      <c r="I10" s="5">
+        <v>22.44</v>
+      </c>
+      <c r="L10" s="10">
+        <f t="shared" si="10"/>
+        <v>62.710038000000011</v>
+      </c>
+      <c r="M10" s="10">
+        <f t="shared" si="6"/>
+        <v>29.760695999999999</v>
+      </c>
+      <c r="N10" s="10">
         <f t="shared" si="2"/>
-        <v>1.7600000000000002</v>
-      </c>
-      <c r="J10" s="6">
-        <f>(D10+E10)/7</f>
-        <v>60000</v>
-      </c>
-      <c r="K10" s="5">
-        <f>SUM(F10:G10)/7</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L10" s="13">
+        <v>1250950.1631634287</v>
+      </c>
+      <c r="O10" s="10">
         <f t="shared" si="7"/>
-        <v>62.710038000000011</v>
-      </c>
-      <c r="M10" s="13">
-        <f t="shared" si="3"/>
-        <v>29.760695999999999</v>
-      </c>
-      <c r="N10" s="13">
-        <f>((H10*L10)+(I10*2*1000*M10))</f>
-        <v>2254816.0956342868</v>
-      </c>
-      <c r="O10" s="13">
-        <f t="shared" si="4"/>
         <v>30.932992000000013</v>
       </c>
-      <c r="P10" s="13">
-        <f t="shared" si="5"/>
+      <c r="P10" s="10">
+        <f t="shared" si="8"/>
         <v>14.680064000000002</v>
       </c>
-      <c r="Q10" s="13">
-        <f t="shared" si="6"/>
-        <v>1112233.5509942863</v>
+      <c r="Q10" s="10">
+        <f t="shared" si="9"/>
+        <v>617056.41749942885</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1238,84 +1242,90 @@
         <v>100</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="D11">
-        <f>D4*B11/10</f>
+        <f>D4*B11/C13</f>
+        <v>50000</v>
+      </c>
+      <c r="E11" s="5">
+        <f>E4*C11/C13</f>
         <v>150000</v>
       </c>
-      <c r="E11">
-        <f>E4*C11/10</f>
-        <v>450000</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f>(C11*C14)*C15*C16*C19*C20/C21</f>
-        <v>13.2</v>
+        <v>67.319999999999993</v>
       </c>
       <c r="G11">
         <f>(C11*C14)*C15*C16*C17*C18/C21</f>
-        <v>33.000000000000007</v>
-      </c>
-      <c r="H11" s="6">
+        <v>168.3</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="4"/>
+        <v>8571.4285714285725</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="5"/>
+        <v>11.220000000000002</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="0"/>
+        <v>28571.428571428572</v>
+      </c>
+      <c r="K11" s="4">
         <f t="shared" si="1"/>
-        <v>25714.28571428571</v>
-      </c>
-      <c r="I11" s="5">
+        <v>33.660000000000004</v>
+      </c>
+      <c r="L11" s="10">
+        <f t="shared" si="10"/>
+        <v>56.439034200000009</v>
+      </c>
+      <c r="M11" s="10">
+        <f t="shared" si="6"/>
+        <v>26.784626400000001</v>
+      </c>
+      <c r="N11" s="10">
         <f t="shared" si="2"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J11" s="6">
-        <f>(D11+E11)/7</f>
-        <v>85714.28571428571</v>
-      </c>
-      <c r="K11" s="5">
-        <f>SUM(F11:G11)/7</f>
-        <v>6.6000000000000005</v>
-      </c>
-      <c r="L11" s="13">
+        <v>1084810.1667017145</v>
+      </c>
+      <c r="O11" s="10">
         <f t="shared" si="7"/>
-        <v>56.439034200000009</v>
-      </c>
-      <c r="M11" s="13">
-        <f t="shared" si="3"/>
-        <v>26.784626400000001</v>
-      </c>
-      <c r="N11" s="13">
-        <f>((H11*L11)+(I11*2*1000*M11))</f>
-        <v>1569141.8070171429</v>
-      </c>
-      <c r="O11" s="13">
-        <f t="shared" si="4"/>
         <v>24.746393600000012</v>
       </c>
-      <c r="P11" s="13">
-        <f t="shared" si="5"/>
+      <c r="P11" s="10">
+        <f t="shared" si="8"/>
         <v>11.744051200000001</v>
       </c>
-      <c r="Q11" s="13">
-        <f t="shared" si="6"/>
-        <v>688009.66070857167</v>
+      <c r="Q11" s="10">
+        <f t="shared" si="9"/>
+        <v>475648.45407085732</v>
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="J12" s="6"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="K13" s="11" t="s">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12">
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9">
         <f>AVERAGE(N5:N11)</f>
-        <v>796861.06527673476</v>
-      </c>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="12">
+        <v>467492.49381746945</v>
+      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="9">
         <f>AVERAGE(Q5:Q11)</f>
-        <v>469593.02697795938</v>
+        <v>257107.13642840827</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1325,13 +1335,13 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
@@ -1340,35 +1350,35 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="C16">
-        <v>1000000</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="12">
+        <v>5100000</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="9">
         <f>AVERAGE(N6:N10)</f>
-        <v>676283.18712685734</v>
-      </c>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="12">
+        <v>469901.94943268568</v>
+      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="9">
         <f>AVERAGE(Q6:Q10)</f>
-        <v>408278.1341988573</v>
+        <v>293597.62589988578</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1378,13 +1388,13 @@
       <c r="C17">
         <v>50000</v>
       </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
@@ -1393,15 +1403,15 @@
       <c r="C18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
@@ -1410,15 +1420,15 @@
       <c r="C19">
         <v>220000</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">

</xml_diff>

<commit_message>
Updated section 1.2 and excel file
</commit_message>
<xml_diff>
--- a/USTier2ComputingProjections.xlsx
+++ b/USTier2ComputingProjections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="-22000" windowWidth="27600" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="6940" yWindow="0" windowWidth="21780" windowHeight="15080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Year</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>2015 resources can be assumed to support 30fb-1</t>
+  </si>
+  <si>
+    <t>We expect that opportunistic resources can provide some of the shortfall, especially in 2016.</t>
   </si>
 </sst>
 </file>
@@ -241,8 +244,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -304,7 +315,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -323,6 +334,10 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -341,6 +356,10 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -670,15 +689,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -803,18 +823,18 @@
         <v>15000</v>
       </c>
       <c r="F4" s="4">
-        <f>(C4+C13)*C15*C16*C19*C20/C21</f>
+        <f>(C4+C14)*C16*C17*C20*C21/C22</f>
         <v>3.8148</v>
       </c>
       <c r="G4" s="4">
-        <f>(C4+C13)*C15*C16*C17*C18/C21</f>
-        <v>9.5370000000000008</v>
+        <f>(C4+C14)*C16*C17*C18*C19/C22</f>
+        <v>13.005000000000001</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
       <c r="J4" s="5">
-        <f>65200/7</f>
-        <v>9314.2857142857138</v>
+        <f>40698/7</f>
+        <v>5814</v>
       </c>
       <c r="K4" s="4">
         <v>2</v>
@@ -846,28 +866,28 @@
         <v>40</v>
       </c>
       <c r="D5">
-        <f>D4*B5/C13</f>
+        <f>D4*B5/C14</f>
         <v>18000</v>
       </c>
       <c r="E5" s="5">
-        <f>E4*C5/C13</f>
+        <f>E4*C5/C14</f>
         <v>20000</v>
       </c>
       <c r="F5" s="5">
-        <f>(C5*C14)*C15*C16*C19*C20/C21</f>
+        <f>(C5*C15)*C16*C17*C20*C21/C22</f>
         <v>8.9760000000000009</v>
       </c>
       <c r="G5">
-        <f>(C5*C14)*C15*C16*C17*C18/C21</f>
-        <v>22.44</v>
+        <f>(C5*C15)*C16*C17*C18*C19/C22</f>
+        <v>30.6</v>
       </c>
       <c r="H5" s="5">
         <f>J5-J4</f>
-        <v>-3885.7142857142853</v>
+        <v>-385.42857142857156</v>
       </c>
       <c r="I5" s="4">
         <f>K5-K4</f>
-        <v>2.4880000000000004</v>
+        <v>3.6537142857142859</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ref="J5:J11" si="0">(D5+E5)/7</f>
@@ -875,7 +895,7 @@
       </c>
       <c r="K5" s="4">
         <f t="shared" ref="K5:K11" si="1">SUM(F5:G5)/7</f>
-        <v>4.4880000000000004</v>
+        <v>5.6537142857142859</v>
       </c>
       <c r="L5" s="10">
         <f>L4*0.9</f>
@@ -887,7 +907,7 @@
       </c>
       <c r="N5" s="10">
         <f t="shared" ref="N5:N11" si="2">((H5*L5)+(I5*2*1000*M5))</f>
-        <v>-161872.45714285705</v>
+        <v>327361.88571428572</v>
       </c>
       <c r="O5" s="10">
         <f>O4*0.8</f>
@@ -899,7 +919,7 @@
       </c>
       <c r="Q5" s="10">
         <f>((H5*O5)+(I5*2*1000*P5))</f>
-        <v>-143886.6285714285</v>
+        <v>290988.34285714291</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -914,20 +934,20 @@
         <v>80</v>
       </c>
       <c r="D6">
-        <f>D4*B6/C13</f>
+        <f>D4*B6/C14</f>
         <v>20000</v>
       </c>
       <c r="E6" s="5">
-        <f>E4*C6/C13</f>
+        <f>E4*C6/C14</f>
         <v>40000</v>
       </c>
       <c r="F6" s="5">
-        <f>(C6*C14)*C15*C16*C19*C20/C21</f>
+        <f>(C6*C15)*C16*C17*C20*C21/C22</f>
         <v>17.952000000000002</v>
       </c>
       <c r="G6">
-        <f>(C6*C14)*C15*C16*C17*C18/C21</f>
-        <v>44.88</v>
+        <f>(C6*C15)*C16*C17*C18*C19/C22</f>
+        <v>61.2</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" ref="H6:H11" si="4">J6-J5</f>
@@ -935,7 +955,7 @@
       </c>
       <c r="I6" s="4">
         <f t="shared" ref="I6:I11" si="5">K6-K5</f>
-        <v>4.4880000000000004</v>
+        <v>5.6537142857142859</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="0"/>
@@ -943,31 +963,31 @@
       </c>
       <c r="K6" s="4">
         <f t="shared" si="1"/>
-        <v>8.9760000000000009</v>
+        <v>11.307428571428572</v>
       </c>
       <c r="L6" s="10">
         <f>L5*0.9</f>
         <v>95.58</v>
       </c>
       <c r="M6" s="10">
-        <f t="shared" ref="M6:M11" si="6">M5*0.9</f>
+        <f t="shared" ref="M6:M12" si="6">M5*0.9</f>
         <v>45.36</v>
       </c>
       <c r="N6" s="10">
         <f t="shared" si="2"/>
-        <v>707545.64571428555</v>
+        <v>813299.24571428564</v>
       </c>
       <c r="O6" s="10">
-        <f t="shared" ref="O6:O11" si="7">O5*0.8</f>
+        <f t="shared" ref="O6:O12" si="7">O5*0.8</f>
         <v>75.52000000000001</v>
       </c>
       <c r="P6" s="10">
-        <f t="shared" ref="P6:P11" si="8">P5*0.8</f>
+        <f t="shared" ref="P6:P12" si="8">P5*0.8</f>
         <v>35.840000000000003</v>
       </c>
       <c r="Q6" s="10">
         <f t="shared" ref="Q6:Q11" si="9">((H6*O6)+(I6*2*1000*P6))</f>
-        <v>559048.41142857145</v>
+        <v>642606.81142857147</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -982,20 +1002,20 @@
         <v>120</v>
       </c>
       <c r="D7">
-        <f>D4*B7/C13</f>
+        <f>D4*B7/C14</f>
         <v>20000</v>
       </c>
       <c r="E7" s="5">
-        <f>E4*C7/C13</f>
+        <f>E4*C7/C14</f>
         <v>60000</v>
       </c>
       <c r="F7" s="5">
-        <f>(C7*C14)*C15*C16*C19*C20/C21</f>
+        <f>(C7*C15)*C16*C17*C20*C21/C22</f>
         <v>26.928000000000001</v>
       </c>
       <c r="G7">
-        <f>(C7*C14)*C15*C16*C17*C18/C21</f>
-        <v>67.320000000000007</v>
+        <f>(C7*C15)*C16*C17*C18*C19/C22</f>
+        <v>91.8</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
@@ -1003,7 +1023,7 @@
       </c>
       <c r="I7" s="4">
         <f t="shared" si="5"/>
-        <v>4.4879999999999995</v>
+        <v>5.653714285714285</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="0"/>
@@ -1011,10 +1031,10 @@
       </c>
       <c r="K7" s="4">
         <f t="shared" si="1"/>
-        <v>13.464</v>
+        <v>16.961142857142857</v>
       </c>
       <c r="L7" s="10">
-        <f t="shared" ref="L7:L11" si="10">L6*0.9</f>
+        <f t="shared" ref="L7:L12" si="10">L6*0.9</f>
         <v>86.022000000000006</v>
       </c>
       <c r="M7" s="10">
@@ -1023,7 +1043,7 @@
       </c>
       <c r="N7" s="10">
         <f t="shared" si="2"/>
-        <v>612213.366857143</v>
+        <v>707391.60685714288</v>
       </c>
       <c r="O7" s="10">
         <f t="shared" si="7"/>
@@ -1035,7 +1055,7 @@
       </c>
       <c r="Q7" s="10">
         <f t="shared" si="9"/>
-        <v>429977.01485714305</v>
+        <v>496823.73485714302</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1050,24 +1070,23 @@
         <v>120</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8" si="11">D7*B8/B7</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E8" s="5">
-        <f>E4*C8/C13</f>
+        <f>E4*C8/C14</f>
         <v>60000</v>
       </c>
       <c r="F8" s="5">
-        <f>(C8*C14)*C15*C16*C19*C20/C21</f>
+        <f>(C8*C15)*C16*C17*C20*C21/C22</f>
         <v>26.928000000000001</v>
       </c>
       <c r="G8">
-        <f>(C8*C14)*C15*C16*C17*C18/C21</f>
-        <v>67.320000000000007</v>
+        <f>(C8*C15)*C16*C17*C18*C19/C22</f>
+        <v>91.8</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>-2857.1428571428587</v>
+        <v>-1428.5714285714294</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="5"/>
@@ -1075,11 +1094,11 @@
       </c>
       <c r="J8" s="5">
         <f t="shared" si="0"/>
-        <v>8571.4285714285706</v>
+        <v>10000</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="1"/>
-        <v>13.464</v>
+        <v>16.961142857142857</v>
       </c>
       <c r="L8" s="10">
         <f t="shared" si="10"/>
@@ -1091,7 +1110,7 @@
       </c>
       <c r="N8" s="10">
         <f t="shared" si="2"/>
-        <v>-221199.42857142873</v>
+        <v>-110599.71428571436</v>
       </c>
       <c r="O8" s="10">
         <f t="shared" si="7"/>
@@ -1103,7 +1122,7 @@
       </c>
       <c r="Q8" s="10">
         <f t="shared" si="9"/>
-        <v>-138093.71428571441</v>
+        <v>-69046.857142857203</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1118,19 +1137,19 @@
         <v>120</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E9" s="5">
-        <f>E4*C9/C13</f>
+        <f>E4*C9/C14</f>
         <v>60000</v>
       </c>
       <c r="F9" s="5">
-        <f>(C9*C14)*C15*C16*C19*C20/C21</f>
+        <f>(C9*C15)*C16*C17*C20*C21/C22</f>
         <v>26.928000000000001</v>
       </c>
       <c r="G9">
-        <f>(C9*C14)*C15*C16*C17*C18/C21</f>
-        <v>67.320000000000007</v>
+        <f>(C9*C15)*C16*C17*C18*C19/C22</f>
+        <v>91.8</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
@@ -1142,11 +1161,11 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" si="0"/>
-        <v>8571.4285714285706</v>
+        <v>10000</v>
       </c>
       <c r="K9" s="4">
         <f t="shared" si="1"/>
-        <v>13.464</v>
+        <v>16.961142857142857</v>
       </c>
       <c r="L9" s="10">
         <f t="shared" si="10"/>
@@ -1178,43 +1197,43 @@
         <v>2021</v>
       </c>
       <c r="B10">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C10">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D10">
-        <f>D4*B10/C13</f>
-        <v>40000</v>
+        <f>D4*B10/C14</f>
+        <v>30000</v>
       </c>
       <c r="E10" s="5">
-        <f>E4*C10/C13</f>
-        <v>100000</v>
+        <f>E4*C10/C14</f>
+        <v>90000</v>
       </c>
       <c r="F10" s="5">
-        <f>(C10*C14)*C15*C16*C19*C20/C21</f>
-        <v>44.88</v>
+        <f>(C10*C15)*C16*C17*C20*C21/C22</f>
+        <v>40.392000000000003</v>
       </c>
       <c r="G10">
-        <f>(C10*C14)*C15*C16*C17*C18/C21</f>
-        <v>112.20000000000002</v>
+        <f>(C10*C15)*C16*C17*C18*C19/C22</f>
+        <v>137.69999999999999</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>11428.571428571429</v>
+        <v>7142.8571428571413</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="5"/>
-        <v>8.9760000000000009</v>
+        <v>8.4805714285714267</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>17142.857142857141</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="1"/>
-        <v>22.44</v>
+        <v>25.441714285714284</v>
       </c>
       <c r="L10" s="10">
         <f t="shared" si="10"/>
@@ -1226,7 +1245,7 @@
       </c>
       <c r="N10" s="10">
         <f t="shared" si="2"/>
-        <v>1250950.1631634287</v>
+        <v>952704.25924114278</v>
       </c>
       <c r="O10" s="10">
         <f t="shared" si="7"/>
@@ -1238,7 +1257,7 @@
       </c>
       <c r="Q10" s="10">
         <f t="shared" si="9"/>
-        <v>617056.41749942885</v>
+        <v>469940.60551314289</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1246,43 +1265,43 @@
         <v>2022</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="D11">
-        <f>D4*B11/C13</f>
-        <v>50000</v>
+        <f>D4*B11/C14</f>
+        <v>30000</v>
       </c>
       <c r="E11" s="5">
-        <f>E4*C11/C13</f>
-        <v>150000</v>
+        <f>E4*C11/C14</f>
+        <v>120000</v>
       </c>
       <c r="F11" s="5">
-        <f>(C11*C14)*C15*C16*C19*C20/C21</f>
-        <v>67.319999999999993</v>
+        <f>(C11*C15)*C16*C17*C20*C21/C22</f>
+        <v>53.856000000000002</v>
       </c>
       <c r="G11">
-        <f>(C11*C14)*C15*C16*C17*C18/C21</f>
-        <v>168.3</v>
+        <f>(C11*C15)*C16*C17*C18*C19/C22</f>
+        <v>183.6</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>8571.4285714285725</v>
+        <v>4285.7142857142862</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="5"/>
-        <v>11.220000000000002</v>
+        <v>8.4805714285714302</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="0"/>
-        <v>28571.428571428572</v>
+        <v>21428.571428571428</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="1"/>
-        <v>33.660000000000004</v>
+        <v>33.922285714285714</v>
       </c>
       <c r="L11" s="10">
         <f t="shared" si="10"/>
@@ -1294,7 +1313,7 @@
       </c>
       <c r="N11" s="10">
         <f t="shared" si="2"/>
-        <v>1084810.1667017145</v>
+        <v>696179.44988845731</v>
       </c>
       <c r="O11" s="10">
         <f t="shared" si="7"/>
@@ -1306,60 +1325,108 @@
       </c>
       <c r="Q11" s="10">
         <f t="shared" si="9"/>
-        <v>475648.45407085732</v>
+        <v>305248.50269622868</v>
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13">
-        <v>30</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9">
-        <f>AVERAGE(N5:N11)</f>
-        <v>467492.49381746945</v>
-      </c>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9">
-        <f>AVERAGE(Q5:Q11)</f>
-        <v>257107.13642840827</v>
+      <c r="A12" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12" si="11">C11+B12</f>
+        <v>300</v>
+      </c>
+      <c r="D12">
+        <f>D4*B12/C14</f>
+        <v>30000</v>
+      </c>
+      <c r="E12" s="5">
+        <f>E4*C12/C14</f>
+        <v>150000</v>
+      </c>
+      <c r="F12" s="5">
+        <f>(C12*C15)*C16*C17*C20*C21/C22</f>
+        <v>67.319999999999993</v>
+      </c>
+      <c r="G12">
+        <f>(C12*C15)*C16*C17*C18*C19/C22</f>
+        <v>229.5</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" ref="H12" si="12">J12-J11</f>
+        <v>4285.7142857142862</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12" si="13">K12-K11</f>
+        <v>8.4805714285714302</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" ref="J12" si="14">(D12+E12)/7</f>
+        <v>25714.285714285714</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" ref="K12" si="15">SUM(F12:G12)/7</f>
+        <v>42.402857142857144</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="10"/>
+        <v>50.795130780000008</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="6"/>
+        <v>24.106163760000001</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" ref="N12" si="16">((H12*L12)+(I12*2*1000*M12))</f>
+        <v>626561.50489961158</v>
+      </c>
+      <c r="O12" s="10">
+        <f t="shared" si="7"/>
+        <v>19.797114880000009</v>
+      </c>
+      <c r="P12" s="10">
+        <f t="shared" si="8"/>
+        <v>9.3952409600000006</v>
+      </c>
+      <c r="Q12" s="10">
+        <f t="shared" ref="Q12" si="17">((H12*O12)+(I12*2*1000*P12))</f>
+        <v>244198.80215698294</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="K14" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
+      <c r="N14" s="9">
+        <f>AVERAGE(N5:N11)</f>
+        <v>483762.39044708572</v>
+      </c>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
+      <c r="Q14" s="9">
+        <f>AVERAGE(Q5:Q11)</f>
+        <v>305223.02002991026</v>
+      </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>40</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -1369,50 +1436,50 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>5100000</v>
-      </c>
-      <c r="K16" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="9">
-        <f>AVERAGE(N6:N10)</f>
-        <v>469901.94943268568</v>
-      </c>
+      <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
-      <c r="Q16" s="9">
-        <f>AVERAGE(Q6:Q10)</f>
-        <v>293597.62589988578</v>
-      </c>
+      <c r="Q16" s="8"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>50000</v>
+        <v>5100000</v>
       </c>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
+      <c r="N17" s="9">
+        <f>AVERAGE(N6:N10)</f>
+        <v>472559.0795053714</v>
+      </c>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="Q17" s="9">
+        <f>AVERAGE(Q6:Q10)</f>
+        <v>308064.8589312</v>
+      </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>41</v>
-      </c>
+        <v>50000</v>
+      </c>
+      <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
@@ -1422,13 +1489,13 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>220000</v>
+        <v>1.5</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -1439,71 +1506,91 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C20">
-        <v>0.1</v>
-      </c>
+        <v>220000</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0.1</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
-      <c r="E23" t="s">
+    <row r="24" spans="1:17">
+      <c r="E24" t="s">
         <v>37</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K24" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K24" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L27" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="E27" t="s">
-        <v>35</v>
-      </c>
-      <c r="L27" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="E29" t="s">
         <v>36</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L29" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>